<commit_message>
Implemented linear->banked memory access for 1MB RAM/ROM card
Fixed bug in max data length return from blockRead - was 1023 now 1024
Fixed length limit on response messages - increased to 5000 bytes
Added unit test for banked memory
</commit_message>
<xml_diff>
--- a/PCB/V2-01/BusRaider V2.01 BOM.xlsx
+++ b/PCB/V2-01/BusRaider V2.01 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RobDev\Projects\Vintage\RC2014\PiBusRaider\PCB\V2-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B1A98E-7B7D-481C-87C7-46516691947C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B373215-5B33-435C-A494-137107307247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26175" yWindow="1950" windowWidth="27570" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25545" yWindow="3150" windowWidth="27570" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -537,6 +537,42 @@
   </si>
   <si>
     <t>https://easyeda.com/robdobsn/busraider-2-01</t>
+  </si>
+  <si>
+    <t>TTGO WEMOS MINI D1 ESP32</t>
+  </si>
+  <si>
+    <t>4814-3004-CP</t>
+  </si>
+  <si>
+    <t>4816-3000-CP</t>
+  </si>
+  <si>
+    <t>4820-3000-CP</t>
+  </si>
+  <si>
+    <t>EasyEDA</t>
+  </si>
+  <si>
+    <t>SanDisk</t>
+  </si>
+  <si>
+    <t>SDSDQAF3-008G-I</t>
+  </si>
+  <si>
+    <t>903-0058-000</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>M1265-2545-N</t>
+  </si>
+  <si>
+    <t>2nd Alt Supplier</t>
+  </si>
+  <si>
+    <t>2nd Alt Supplier Part</t>
   </si>
 </sst>
 </file>
@@ -996,11 +1032,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1056,7 @@
     <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1057,8 +1093,14 @@
       <c r="L1" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1081,22 +1123,22 @@
         <v>26</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="6">
-        <v>1749756</v>
+        <v>31</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1749756</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1119,22 +1161,22 @@
         <v>26</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1470786</v>
+        <v>31</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="L3" s="6">
+        <v>1470786</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1157,22 +1199,22 @@
         <v>26</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="6">
-        <v>9591664</v>
+        <v>31</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="L4" s="6">
+        <v>9591664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1203,9 +1245,8 @@
       <c r="J5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1227,23 +1268,23 @@
       <c r="G6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1470803</v>
+      <c r="H6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1470803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1266,22 +1307,22 @@
         <v>26</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1105965</v>
+        <v>31</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="L7" s="6">
+        <v>1105965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1303,23 +1344,23 @@
       <c r="G8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1470823</v>
+      <c r="H8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="6">
+        <v>1470823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1342,22 +1383,22 @@
         <v>26</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1105963</v>
+        <v>31</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1105963</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1380,16 +1421,22 @@
         <v>68</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="6">
-        <v>2445624</v>
+        <v>31</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="6">
+        <v>2445624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1412,16 +1459,22 @@
         <v>68</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="6">
-        <v>2445622</v>
+        <v>31</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="6">
+        <v>2445622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1432,7 +1485,7 @@
         <v>87</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E12" s="5">
         <v>5</v>
@@ -1444,16 +1497,22 @@
         <v>68</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="6">
-        <v>2445621</v>
+        <v>31</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="6">
+        <v>2445621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1476,22 +1535,22 @@
         <v>79</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="6">
-        <v>2554986</v>
+        <v>31</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="L13" s="6">
+        <v>2554986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1507,17 +1566,23 @@
       <c r="E14" s="5">
         <v>1</v>
       </c>
+      <c r="F14" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="G14" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="J14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="N14" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1549,7 +1614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2114,7 +2179,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -2125,7 +2190,7 @@
         <v>158</v>
       </c>
       <c r="E33" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>160</v>
@@ -2140,7 +2205,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -2148,14 +2213,22 @@
         <v>162</v>
       </c>
       <c r="E34" s="5">
-        <v>3</v>
-      </c>
-      <c r="I34" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="J34" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2163,15 +2236,20 @@
         <v>166</v>
       </c>
       <c r="E35" s="5">
-        <v>3</v>
-      </c>
-      <c r="I35" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="J35" s="5" t="s">
         <v>39</v>
       </c>
       <c r="K35" s="6"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -2183,11 +2261,23 @@
       <c r="E36" s="7">
         <v>1</v>
       </c>
+      <c r="F36" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="J36" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -2197,56 +2287,54 @@
       <c r="E37" s="5">
         <v>1</v>
       </c>
-      <c r="I37" s="6" t="s">
+      <c r="M37" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="N37" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I38" s="6"/>
       <c r="K38" s="6"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F41" s="11"/>
       <c r="I41" s="3"/>
       <c r="K41" s="9"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F42" s="11"/>
       <c r="I42" s="6"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I43" s="6"/>
       <c r="K43" s="9"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I45" s="8"/>
-      <c r="K45" s="9"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I46" s="6"/>
-      <c r="K46" s="9"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I47" s="6"/>
-      <c r="K47" s="9"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I48" s="6"/>
-      <c r="K48" s="6"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I49" s="6"/>
-      <c r="K49" s="9"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
@@ -2257,8 +2345,6 @@
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="6"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="6"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
@@ -2269,8 +2355,6 @@
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="6"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="9"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
@@ -2313,27 +2397,27 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" tooltip="1749756" display="http://uk.farnell.com/texas-instruments/sn74lvc245an/logic-bus-transcvr-octal-20dip/dp/1749756?st=74lvc245" xr:uid="{47D6DFA3-1F3A-41A6-A358-D96BCCE25372}"/>
-    <hyperlink ref="I10" r:id="rId2" tooltip="2445624" display="https://uk.farnell.com/te-connectivity/1-2199298-6/ic-socket-dip-20pos-th/dp/2445624?st=ic%20socket%2020" xr:uid="{5E1E66B2-FB50-427F-8BB8-147C0BBC0035}"/>
-    <hyperlink ref="I3" r:id="rId3" tooltip="1470786" display="http://uk.farnell.com/texas-instruments/sn74hc590an/ic-counter-binary/dp/1470786?st=74hc590" xr:uid="{6C1D994B-934B-4328-85E0-1377F07D38C1}"/>
-    <hyperlink ref="I11" r:id="rId4" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{F5822B7C-9CD8-47AD-BE52-137426BF87E1}"/>
-    <hyperlink ref="I4" r:id="rId5" tooltip="9591664" display="http://uk.farnell.com/texas-instruments/sn74hc595n/shift-register-8bit-74hc595-dip16/dp/9591664?st=74hc595" xr:uid="{8C022005-98E9-4D11-B8E8-913686A5E95F}"/>
-    <hyperlink ref="I6" r:id="rId6" display="https://uk.farnell.com/texas-instruments/sn74hct138n/ic-decoder-demux/dp/1470803" xr:uid="{0B351759-0094-448B-BA57-F9E6CA50ED0E}"/>
-    <hyperlink ref="L2" r:id="rId7" xr:uid="{B3BD62FB-3DB9-44ED-971A-3D67E511F547}"/>
-    <hyperlink ref="L3" r:id="rId8" xr:uid="{78458766-1E42-4DFB-83EB-63FF215095C9}"/>
-    <hyperlink ref="L6" r:id="rId9" xr:uid="{436D0B18-7AD3-4B69-BBF9-5A18820A8E7E}"/>
-    <hyperlink ref="L8" r:id="rId10" display="https://www.mouser.co.uk/ProductDetail/595-SN74HCT74N" xr:uid="{BB7198B6-1E8E-4679-9979-3FA32835E852}"/>
-    <hyperlink ref="L4" r:id="rId11" xr:uid="{0BDD3D75-51CE-429D-A46E-5A2D63044A7C}"/>
+    <hyperlink ref="L2" r:id="rId1" tooltip="1749756" display="http://uk.farnell.com/texas-instruments/sn74lvc245an/logic-bus-transcvr-octal-20dip/dp/1749756?st=74lvc245" xr:uid="{47D6DFA3-1F3A-41A6-A358-D96BCCE25372}"/>
+    <hyperlink ref="L10" r:id="rId2" tooltip="2445624" display="https://uk.farnell.com/te-connectivity/1-2199298-6/ic-socket-dip-20pos-th/dp/2445624?st=ic%20socket%2020" xr:uid="{5E1E66B2-FB50-427F-8BB8-147C0BBC0035}"/>
+    <hyperlink ref="L3" r:id="rId3" tooltip="1470786" display="http://uk.farnell.com/texas-instruments/sn74hc590an/ic-counter-binary/dp/1470786?st=74hc590" xr:uid="{6C1D994B-934B-4328-85E0-1377F07D38C1}"/>
+    <hyperlink ref="L11" r:id="rId4" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{F5822B7C-9CD8-47AD-BE52-137426BF87E1}"/>
+    <hyperlink ref="L4" r:id="rId5" tooltip="9591664" display="http://uk.farnell.com/texas-instruments/sn74hc595n/shift-register-8bit-74hc595-dip16/dp/9591664?st=74hc595" xr:uid="{8C022005-98E9-4D11-B8E8-913686A5E95F}"/>
+    <hyperlink ref="L6" r:id="rId6" display="https://uk.farnell.com/texas-instruments/sn74hct138n/ic-decoder-demux/dp/1470803" xr:uid="{0B351759-0094-448B-BA57-F9E6CA50ED0E}"/>
+    <hyperlink ref="I2" r:id="rId7" xr:uid="{B3BD62FB-3DB9-44ED-971A-3D67E511F547}"/>
+    <hyperlink ref="I3" r:id="rId8" xr:uid="{78458766-1E42-4DFB-83EB-63FF215095C9}"/>
+    <hyperlink ref="I6" r:id="rId9" xr:uid="{436D0B18-7AD3-4B69-BBF9-5A18820A8E7E}"/>
+    <hyperlink ref="I8" r:id="rId10" display="https://www.mouser.co.uk/ProductDetail/595-SN74HCT74N" xr:uid="{BB7198B6-1E8E-4679-9979-3FA32835E852}"/>
+    <hyperlink ref="I4" r:id="rId11" xr:uid="{0BDD3D75-51CE-429D-A46E-5A2D63044A7C}"/>
     <hyperlink ref="I5" r:id="rId12" xr:uid="{D505C044-4022-48F3-9CA6-843831FB61C8}"/>
-    <hyperlink ref="I13" r:id="rId13" tooltip="2554986" display="https://uk.farnell.com/stmicroelectronics/l4931cz33-ap/ldo-fixed-3-3v-0-25a-to-92-3/dp/2554986?st=L4931CZ33-AP" xr:uid="{3E2F7914-9F59-4B57-B734-649737FDD89E}"/>
-    <hyperlink ref="L13" r:id="rId14" xr:uid="{D23C02A9-30FB-447C-B6B6-FFDD00EC9EF5}"/>
-    <hyperlink ref="I7" r:id="rId15" tooltip="1105965" display="https://uk.farnell.com/texas-instruments/cd74hct08e/74hct-cmos-74hct08-dip14-5-5v/dp/1105965?st=cd74hct08" xr:uid="{C77AB365-4AE3-4151-B697-50EEA6F2DB2B}"/>
-    <hyperlink ref="L7" r:id="rId16" xr:uid="{B934DA2C-C18C-44E7-8FAA-8475F89B0FA2}"/>
-    <hyperlink ref="I8" r:id="rId17" display="https://uk.farnell.com/texas-instruments/sn74hct74n/ic-flip-flop-2-circuits/dp/1470823?MER=sy-me-pd-mi-alte&amp;st=74hct74" xr:uid="{5750A802-3DD7-4FD1-BA5B-66CBCED46A4F}"/>
-    <hyperlink ref="I14" r:id="rId18" xr:uid="{3DD78D9F-009C-445B-A736-1DB8D0E28886}"/>
-    <hyperlink ref="I9" r:id="rId19" display="https://uk.farnell.com/texas-instruments/cd74hct02e/74hct-cmos-74hct02-dip14-5-5v/dp/1105963" xr:uid="{BA8E576B-AD87-409B-B1D4-96BD0C7B4C8F}"/>
-    <hyperlink ref="L9" r:id="rId20" xr:uid="{16D7E5E3-3D9F-4F2F-A8C5-44D2B59E8DF3}"/>
-    <hyperlink ref="I12" r:id="rId21" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{E62CAF29-57B4-4B92-8383-203B6BDF7508}"/>
+    <hyperlink ref="L13" r:id="rId13" tooltip="2554986" display="https://uk.farnell.com/stmicroelectronics/l4931cz33-ap/ldo-fixed-3-3v-0-25a-to-92-3/dp/2554986?st=L4931CZ33-AP" xr:uid="{3E2F7914-9F59-4B57-B734-649737FDD89E}"/>
+    <hyperlink ref="I13" r:id="rId14" xr:uid="{D23C02A9-30FB-447C-B6B6-FFDD00EC9EF5}"/>
+    <hyperlink ref="L7" r:id="rId15" tooltip="1105965" display="https://uk.farnell.com/texas-instruments/cd74hct08e/74hct-cmos-74hct08-dip14-5-5v/dp/1105965?st=cd74hct08" xr:uid="{C77AB365-4AE3-4151-B697-50EEA6F2DB2B}"/>
+    <hyperlink ref="I7" r:id="rId16" xr:uid="{B934DA2C-C18C-44E7-8FAA-8475F89B0FA2}"/>
+    <hyperlink ref="L8" r:id="rId17" display="https://uk.farnell.com/texas-instruments/sn74hct74n/ic-flip-flop-2-circuits/dp/1470823?MER=sy-me-pd-mi-alte&amp;st=74hct74" xr:uid="{5750A802-3DD7-4FD1-BA5B-66CBCED46A4F}"/>
+    <hyperlink ref="N14" r:id="rId18" xr:uid="{3DD78D9F-009C-445B-A736-1DB8D0E28886}"/>
+    <hyperlink ref="L9" r:id="rId19" display="https://uk.farnell.com/texas-instruments/cd74hct02e/74hct-cmos-74hct02-dip14-5-5v/dp/1105963" xr:uid="{BA8E576B-AD87-409B-B1D4-96BD0C7B4C8F}"/>
+    <hyperlink ref="I9" r:id="rId20" xr:uid="{16D7E5E3-3D9F-4F2F-A8C5-44D2B59E8DF3}"/>
+    <hyperlink ref="L12" r:id="rId21" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{E62CAF29-57B4-4B92-8383-203B6BDF7508}"/>
     <hyperlink ref="I15" r:id="rId22" xr:uid="{20220901-2B6D-40CB-B181-FFB0720BAB8E}"/>
     <hyperlink ref="I16" r:id="rId23" xr:uid="{986AD98A-B980-40AE-9E81-BD3EB1E1CCA4}"/>
     <hyperlink ref="I17" r:id="rId24" xr:uid="{4DD6EB77-35D1-4B71-9401-D0238A04D669}"/>
@@ -2357,8 +2441,14 @@
     <hyperlink ref="I28" r:id="rId42" xr:uid="{2F348C2D-AF2B-4DF9-8037-9842338891DE}"/>
     <hyperlink ref="I33" r:id="rId43" xr:uid="{9BFEF78D-6B49-4504-8ADB-FC6453F0A13A}"/>
     <hyperlink ref="I32" r:id="rId44" xr:uid="{6BFCB960-4BC4-4AE7-84CC-EF1CFA05B512}"/>
+    <hyperlink ref="I12" r:id="rId45" tooltip="Click to view additional information on this product." xr:uid="{D073EBC7-F736-4CCE-9903-05965C4089DE}"/>
+    <hyperlink ref="I11" r:id="rId46" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/3M-Electronic-Solutions-Division/4816-3000-CP?qs=sGAEpiMZZMs%2FSh%2Fkjph1tvt1%2FmEPT%2FXo2MaLGaLrmns%3D" xr:uid="{110F6884-1DF7-4F57-806C-4EDE39B930B4}"/>
+    <hyperlink ref="I10" r:id="rId47" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/3M-Electronic-Solutions-Division/4820-3000-CP?qs=sGAEpiMZZMs%2FSh%2Fkjph1tvt1%2FmEPT%2FXoGLwqMMa088g%3D" xr:uid="{19C30A73-5D3F-4B86-8369-F9B8DC755041}"/>
+    <hyperlink ref="I36" r:id="rId48" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/SanDisk/SDSDQAF3-008G-I?qs=sGAEpiMZZMtyMAXUUxCBE5IlUgcznewuII5iIueKP0p3215DGin%2Fpg%3D%3D" xr:uid="{1EADA45E-12D0-466C-97A1-D43608EB28DD}"/>
+    <hyperlink ref="I35" r:id="rId49" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/ROBOTIS/903-0058-000?qs=sGAEpiMZZMve4%2FbfQkoj%252BAsyQJpshgj7rMaVzceycow%3D" xr:uid="{81304EC3-CBD1-42AA-9761-BC59FFC325EE}"/>
+    <hyperlink ref="I34" r:id="rId50" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/RAF-Electronic-Hardware/M1265-2545-N?qs=sGAEpiMZZMv2WiXdFcmpiEsCM5xSt%2Fxk" xr:uid="{5D20D5BB-959D-47FB-870B-95BC22A83998}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId45"/>
+  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM for V2.01
</commit_message>
<xml_diff>
--- a/PCB/V2-01/BusRaider V2.01 BOM.xlsx
+++ b/PCB/V2-01/BusRaider V2.01 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RobDev\Projects\Vintage\RC2014\PiBusRaider\PCB\V2-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B373215-5B33-435C-A494-137107307247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4F705D-589F-4E70-AD4D-9F6BF01B72D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25545" yWindow="3150" windowWidth="27570" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10545" yWindow="3810" windowWidth="29340" windowHeight="17535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="185">
   <si>
     <t>ID</t>
   </si>
@@ -272,9 +272,6 @@
     <t>511-L4931CZ33-AP</t>
   </si>
   <si>
-    <t>U10,U13</t>
-  </si>
-  <si>
     <t>WEMOS D1 MINI ESP32</t>
   </si>
   <si>
@@ -573,13 +570,25 @@
   </si>
   <si>
     <t>2nd Alt Supplier Part</t>
+  </si>
+  <si>
+    <t>74HC74N</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>U13</t>
+  </si>
+  <si>
+    <t>595-SN74HC74N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -648,6 +657,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -686,7 +701,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -723,6 +738,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1032,11 +1050,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,10 +1112,10 @@
         <v>66</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1327,19 +1345,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>81</v>
+        <v>182</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>74</v>
       </c>
       <c r="E8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>38</v>
+        <v>181</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>26</v>
@@ -1348,7 +1366,7 @@
         <v>31</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>53</v>
+        <v>184</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>39</v>
@@ -1356,104 +1374,104 @@
       <c r="K8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="6">
-        <v>1470823</v>
+      <c r="L8" s="16">
+        <v>9591699</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="6">
+        <v>1470823</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="H10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="6">
-        <v>1105963</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="5">
-        <v>4</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="L10" s="6">
-        <v>2445624</v>
+        <v>1105963</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E11" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>68</v>
@@ -1471,27 +1489,27 @@
         <v>25</v>
       </c>
       <c r="L11" s="6">
-        <v>2445622</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2445624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E12" s="5">
-        <v>5</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>90</v>
+        <v>3</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>68</v>
@@ -1509,36 +1527,36 @@
         <v>25</v>
       </c>
       <c r="L12" s="6">
-        <v>2445621</v>
+        <v>2445622</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>78</v>
+        <v>5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>80</v>
+      <c r="I13" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>10</v>
@@ -1547,47 +1565,53 @@
         <v>25</v>
       </c>
       <c r="L13" s="6">
-        <v>2554986</v>
+        <v>2445621</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>170</v>
+        <v>78</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>85</v>
+        <v>10</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="6">
+        <v>2554986</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>34</v>
@@ -1598,49 +1622,49 @@
       <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>96</v>
+      <c r="F15" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>95</v>
+      <c r="I16" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>10</v>
@@ -1648,22 +1672,22 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>22</v>
@@ -1672,7 +1696,7 @@
         <v>31</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>10</v>
@@ -1680,19 +1704,19 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E18" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>104</v>
@@ -1704,7 +1728,7 @@
         <v>31</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>10</v>
@@ -1712,31 +1736,31 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E19" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>10</v>
@@ -1744,168 +1768,168 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
       </c>
-      <c r="F20" s="5">
-        <v>5033981892</v>
+      <c r="F20" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K20" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="12">
-        <v>2358234</v>
-      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E21" s="5">
-        <v>5</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>5033981892</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="L21" s="12">
+        <v>2358234</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>48</v>
+        <v>5</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="6">
-        <v>2889133</v>
+        <v>21</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>125</v>
+        <v>48</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>29</v>
+      <c r="F23" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="K23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="6">
+        <v>2889133</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>30</v>
@@ -1914,7 +1938,7 @@
         <v>31</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
       <c r="J24" s="5" t="s">
         <v>10</v>
@@ -1922,13 +1946,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>123</v>
@@ -1937,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>30</v>
@@ -1946,7 +1970,7 @@
         <v>31</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="J25" s="5" t="s">
         <v>10</v>
@@ -1954,102 +1978,101 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>131</v>
+        <v>47</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>141</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L27" s="6"/>
+      <c r="K27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>157</v>
+        <v>9</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="E28" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>10</v>
@@ -2058,31 +2081,31 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>141</v>
+        <v>152</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="E29" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>10</v>
@@ -2091,45 +2114,46 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>117</v>
+        <v>144</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>116</v>
+      <c r="I30" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="J30" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>146</v>
@@ -2137,17 +2161,17 @@
       <c r="E31" s="5">
         <v>1</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>150</v>
+      <c r="F31" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I31" s="12" t="s">
-        <v>151</v>
+      <c r="I31" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>10</v>
@@ -2155,51 +2179,57 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>163</v>
+        <v>147</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="E32" s="5">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J32" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E33" s="5">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>31</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>39</v>
@@ -2207,22 +2237,25 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>157</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
       </c>
       <c r="G34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="J34" s="5" t="s">
         <v>39</v>
@@ -2230,45 +2263,39 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E35" s="5">
         <v>1</v>
       </c>
       <c r="G35" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="J35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K35" s="6"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>35</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7">
-        <v>1</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>176</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="5">
+        <v>1</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>31</v>
+        <v>177</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>176</v>
@@ -2276,56 +2303,82 @@
       <c r="J36" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="K36" s="6"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" s="5">
+        <v>1</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="N38" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E37" s="5">
-        <v>1</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="N37" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I38" s="6"/>
-      <c r="K38" s="6"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I39" s="6"/>
+      <c r="K39" s="6"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F41" s="11"/>
-      <c r="I41" s="3"/>
-      <c r="K41" s="9"/>
+      <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F42" s="11"/>
-      <c r="I42" s="6"/>
+      <c r="I42" s="3"/>
       <c r="K42" s="9"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F43" s="11"/>
       <c r="I43" s="6"/>
       <c r="K43" s="9"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I44" s="6"/>
+      <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I45" s="8"/>
+      <c r="I45" s="6"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I46" s="6"/>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I47" s="6"/>
@@ -2337,13 +2390,6 @@
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
@@ -2365,26 +2411,27 @@
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="6"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="9"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
       <c r="I53" s="6"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="9"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I54" s="8"/>
+      <c r="I54" s="6"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="I55" s="6"/>
+      <c r="I55" s="8"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="7"/>
+      <c r="I56" s="6"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
@@ -2392,63 +2439,73 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
+      <c r="I57" s="8"/>
       <c r="J57" s="7"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="J58" s="7"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" tooltip="1749756" display="http://uk.farnell.com/texas-instruments/sn74lvc245an/logic-bus-transcvr-octal-20dip/dp/1749756?st=74lvc245" xr:uid="{47D6DFA3-1F3A-41A6-A358-D96BCCE25372}"/>
-    <hyperlink ref="L10" r:id="rId2" tooltip="2445624" display="https://uk.farnell.com/te-connectivity/1-2199298-6/ic-socket-dip-20pos-th/dp/2445624?st=ic%20socket%2020" xr:uid="{5E1E66B2-FB50-427F-8BB8-147C0BBC0035}"/>
+    <hyperlink ref="L11" r:id="rId2" tooltip="2445624" display="https://uk.farnell.com/te-connectivity/1-2199298-6/ic-socket-dip-20pos-th/dp/2445624?st=ic%20socket%2020" xr:uid="{5E1E66B2-FB50-427F-8BB8-147C0BBC0035}"/>
     <hyperlink ref="L3" r:id="rId3" tooltip="1470786" display="http://uk.farnell.com/texas-instruments/sn74hc590an/ic-counter-binary/dp/1470786?st=74hc590" xr:uid="{6C1D994B-934B-4328-85E0-1377F07D38C1}"/>
-    <hyperlink ref="L11" r:id="rId4" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{F5822B7C-9CD8-47AD-BE52-137426BF87E1}"/>
+    <hyperlink ref="L12" r:id="rId4" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{F5822B7C-9CD8-47AD-BE52-137426BF87E1}"/>
     <hyperlink ref="L4" r:id="rId5" tooltip="9591664" display="http://uk.farnell.com/texas-instruments/sn74hc595n/shift-register-8bit-74hc595-dip16/dp/9591664?st=74hc595" xr:uid="{8C022005-98E9-4D11-B8E8-913686A5E95F}"/>
     <hyperlink ref="L6" r:id="rId6" display="https://uk.farnell.com/texas-instruments/sn74hct138n/ic-decoder-demux/dp/1470803" xr:uid="{0B351759-0094-448B-BA57-F9E6CA50ED0E}"/>
     <hyperlink ref="I2" r:id="rId7" xr:uid="{B3BD62FB-3DB9-44ED-971A-3D67E511F547}"/>
     <hyperlink ref="I3" r:id="rId8" xr:uid="{78458766-1E42-4DFB-83EB-63FF215095C9}"/>
     <hyperlink ref="I6" r:id="rId9" xr:uid="{436D0B18-7AD3-4B69-BBF9-5A18820A8E7E}"/>
-    <hyperlink ref="I8" r:id="rId10" display="https://www.mouser.co.uk/ProductDetail/595-SN74HCT74N" xr:uid="{BB7198B6-1E8E-4679-9979-3FA32835E852}"/>
+    <hyperlink ref="I9" r:id="rId10" display="https://www.mouser.co.uk/ProductDetail/595-SN74HCT74N" xr:uid="{BB7198B6-1E8E-4679-9979-3FA32835E852}"/>
     <hyperlink ref="I4" r:id="rId11" xr:uid="{0BDD3D75-51CE-429D-A46E-5A2D63044A7C}"/>
     <hyperlink ref="I5" r:id="rId12" xr:uid="{D505C044-4022-48F3-9CA6-843831FB61C8}"/>
-    <hyperlink ref="L13" r:id="rId13" tooltip="2554986" display="https://uk.farnell.com/stmicroelectronics/l4931cz33-ap/ldo-fixed-3-3v-0-25a-to-92-3/dp/2554986?st=L4931CZ33-AP" xr:uid="{3E2F7914-9F59-4B57-B734-649737FDD89E}"/>
-    <hyperlink ref="I13" r:id="rId14" xr:uid="{D23C02A9-30FB-447C-B6B6-FFDD00EC9EF5}"/>
+    <hyperlink ref="L14" r:id="rId13" tooltip="2554986" display="https://uk.farnell.com/stmicroelectronics/l4931cz33-ap/ldo-fixed-3-3v-0-25a-to-92-3/dp/2554986?st=L4931CZ33-AP" xr:uid="{3E2F7914-9F59-4B57-B734-649737FDD89E}"/>
+    <hyperlink ref="I14" r:id="rId14" xr:uid="{D23C02A9-30FB-447C-B6B6-FFDD00EC9EF5}"/>
     <hyperlink ref="L7" r:id="rId15" tooltip="1105965" display="https://uk.farnell.com/texas-instruments/cd74hct08e/74hct-cmos-74hct08-dip14-5-5v/dp/1105965?st=cd74hct08" xr:uid="{C77AB365-4AE3-4151-B697-50EEA6F2DB2B}"/>
     <hyperlink ref="I7" r:id="rId16" xr:uid="{B934DA2C-C18C-44E7-8FAA-8475F89B0FA2}"/>
-    <hyperlink ref="L8" r:id="rId17" display="https://uk.farnell.com/texas-instruments/sn74hct74n/ic-flip-flop-2-circuits/dp/1470823?MER=sy-me-pd-mi-alte&amp;st=74hct74" xr:uid="{5750A802-3DD7-4FD1-BA5B-66CBCED46A4F}"/>
-    <hyperlink ref="N14" r:id="rId18" xr:uid="{3DD78D9F-009C-445B-A736-1DB8D0E28886}"/>
-    <hyperlink ref="L9" r:id="rId19" display="https://uk.farnell.com/texas-instruments/cd74hct02e/74hct-cmos-74hct02-dip14-5-5v/dp/1105963" xr:uid="{BA8E576B-AD87-409B-B1D4-96BD0C7B4C8F}"/>
-    <hyperlink ref="I9" r:id="rId20" xr:uid="{16D7E5E3-3D9F-4F2F-A8C5-44D2B59E8DF3}"/>
-    <hyperlink ref="L12" r:id="rId21" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{E62CAF29-57B4-4B92-8383-203B6BDF7508}"/>
-    <hyperlink ref="I15" r:id="rId22" xr:uid="{20220901-2B6D-40CB-B181-FFB0720BAB8E}"/>
-    <hyperlink ref="I16" r:id="rId23" xr:uid="{986AD98A-B980-40AE-9E81-BD3EB1E1CCA4}"/>
-    <hyperlink ref="I17" r:id="rId24" xr:uid="{4DD6EB77-35D1-4B71-9401-D0238A04D669}"/>
-    <hyperlink ref="I18" r:id="rId25" xr:uid="{F5E17176-3AC5-483E-88AA-26B30E4AC82D}"/>
-    <hyperlink ref="I20" r:id="rId26" xr:uid="{464D5325-DA76-4039-BC35-6AB9A231F364}"/>
-    <hyperlink ref="I19" r:id="rId27" xr:uid="{8E91D5C6-D213-4807-8B3D-D56007AA1559}"/>
-    <hyperlink ref="L21" r:id="rId28" display="https://uk.rs-online.com/web/p/mosfet-transistors/6714736/" xr:uid="{DE5C3F69-D9BA-45F4-827E-D4750CC0CC5E}"/>
-    <hyperlink ref="I21" r:id="rId29" xr:uid="{1BFFA011-DA50-46C1-95BC-C4AAB7E00104}"/>
-    <hyperlink ref="I30" r:id="rId30" xr:uid="{601F6E5C-F79C-438B-B10A-1985178E169F}"/>
-    <hyperlink ref="I24" r:id="rId31" xr:uid="{F1E33841-2CB6-4061-86BC-958A61D713BE}"/>
-    <hyperlink ref="I23" r:id="rId32" xr:uid="{D635069F-892A-4F1F-8550-500CBD57C42A}"/>
-    <hyperlink ref="L22" r:id="rId33" tooltip="2889133" display="https://uk.farnell.com/vishay/bat85s-tap/diode-schottky-aec-q101-30v-do/dp/2889133?st=bat85" xr:uid="{18F3B860-1AAD-4C5B-BD94-B85954AE7BCF}"/>
-    <hyperlink ref="I25" r:id="rId34" xr:uid="{B2EB5659-CB87-4BB3-8D5A-9C7B2409CC19}"/>
-    <hyperlink ref="I22" r:id="rId35" xr:uid="{2BA0131D-28BF-4B2D-98A8-13B8FD5B1EF5}"/>
-    <hyperlink ref="L20" r:id="rId36" display="https://uk.farnell.com/molex/503398-1892/connector-micro-sd-8pos/dp/2358234?st=5033981892" xr:uid="{11D74044-851C-44EA-91AC-722C6CFB6B3E}"/>
-    <hyperlink ref="I26" r:id="rId37" xr:uid="{2D1FA75B-D9CA-4B13-9AB8-0C3547D07D4A}"/>
-    <hyperlink ref="L26" r:id="rId38" xr:uid="{6CE39B34-9E28-4E0B-8AFF-04670F4E0343}"/>
-    <hyperlink ref="I29" r:id="rId39" xr:uid="{35148EC9-0BBC-4B0C-AAFE-047F71F4E110}"/>
-    <hyperlink ref="I27" r:id="rId40" xr:uid="{AE824952-DBA2-482B-9BC1-1C60443820F2}"/>
-    <hyperlink ref="I31" r:id="rId41" xr:uid="{3DF2667A-C25F-4862-BD28-16FE9FB53834}"/>
-    <hyperlink ref="I28" r:id="rId42" xr:uid="{2F348C2D-AF2B-4DF9-8037-9842338891DE}"/>
-    <hyperlink ref="I33" r:id="rId43" xr:uid="{9BFEF78D-6B49-4504-8ADB-FC6453F0A13A}"/>
-    <hyperlink ref="I32" r:id="rId44" xr:uid="{6BFCB960-4BC4-4AE7-84CC-EF1CFA05B512}"/>
-    <hyperlink ref="I12" r:id="rId45" tooltip="Click to view additional information on this product." xr:uid="{D073EBC7-F736-4CCE-9903-05965C4089DE}"/>
-    <hyperlink ref="I11" r:id="rId46" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/3M-Electronic-Solutions-Division/4816-3000-CP?qs=sGAEpiMZZMs%2FSh%2Fkjph1tvt1%2FmEPT%2FXo2MaLGaLrmns%3D" xr:uid="{110F6884-1DF7-4F57-806C-4EDE39B930B4}"/>
-    <hyperlink ref="I10" r:id="rId47" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/3M-Electronic-Solutions-Division/4820-3000-CP?qs=sGAEpiMZZMs%2FSh%2Fkjph1tvt1%2FmEPT%2FXoGLwqMMa088g%3D" xr:uid="{19C30A73-5D3F-4B86-8369-F9B8DC755041}"/>
-    <hyperlink ref="I36" r:id="rId48" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/SanDisk/SDSDQAF3-008G-I?qs=sGAEpiMZZMtyMAXUUxCBE5IlUgcznewuII5iIueKP0p3215DGin%2Fpg%3D%3D" xr:uid="{1EADA45E-12D0-466C-97A1-D43608EB28DD}"/>
-    <hyperlink ref="I35" r:id="rId49" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/ROBOTIS/903-0058-000?qs=sGAEpiMZZMve4%2FbfQkoj%252BAsyQJpshgj7rMaVzceycow%3D" xr:uid="{81304EC3-CBD1-42AA-9761-BC59FFC325EE}"/>
-    <hyperlink ref="I34" r:id="rId50" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/RAF-Electronic-Hardware/M1265-2545-N?qs=sGAEpiMZZMv2WiXdFcmpiEsCM5xSt%2Fxk" xr:uid="{5D20D5BB-959D-47FB-870B-95BC22A83998}"/>
+    <hyperlink ref="N15" r:id="rId17" xr:uid="{3DD78D9F-009C-445B-A736-1DB8D0E28886}"/>
+    <hyperlink ref="L10" r:id="rId18" display="https://uk.farnell.com/texas-instruments/cd74hct02e/74hct-cmos-74hct02-dip14-5-5v/dp/1105963" xr:uid="{BA8E576B-AD87-409B-B1D4-96BD0C7B4C8F}"/>
+    <hyperlink ref="I10" r:id="rId19" xr:uid="{16D7E5E3-3D9F-4F2F-A8C5-44D2B59E8DF3}"/>
+    <hyperlink ref="L13" r:id="rId20" tooltip="2445622" display="https://uk.farnell.com/te-connectivity/1-2199298-4/ic-socket-dip-16pos-th/dp/2445622?st=ic%20socket%2016" xr:uid="{E62CAF29-57B4-4B92-8383-203B6BDF7508}"/>
+    <hyperlink ref="I16" r:id="rId21" xr:uid="{20220901-2B6D-40CB-B181-FFB0720BAB8E}"/>
+    <hyperlink ref="I17" r:id="rId22" xr:uid="{986AD98A-B980-40AE-9E81-BD3EB1E1CCA4}"/>
+    <hyperlink ref="I18" r:id="rId23" xr:uid="{4DD6EB77-35D1-4B71-9401-D0238A04D669}"/>
+    <hyperlink ref="I19" r:id="rId24" xr:uid="{F5E17176-3AC5-483E-88AA-26B30E4AC82D}"/>
+    <hyperlink ref="I21" r:id="rId25" xr:uid="{464D5325-DA76-4039-BC35-6AB9A231F364}"/>
+    <hyperlink ref="I20" r:id="rId26" xr:uid="{8E91D5C6-D213-4807-8B3D-D56007AA1559}"/>
+    <hyperlink ref="L22" r:id="rId27" display="https://uk.rs-online.com/web/p/mosfet-transistors/6714736/" xr:uid="{DE5C3F69-D9BA-45F4-827E-D4750CC0CC5E}"/>
+    <hyperlink ref="I22" r:id="rId28" xr:uid="{1BFFA011-DA50-46C1-95BC-C4AAB7E00104}"/>
+    <hyperlink ref="I31" r:id="rId29" xr:uid="{601F6E5C-F79C-438B-B10A-1985178E169F}"/>
+    <hyperlink ref="I25" r:id="rId30" xr:uid="{F1E33841-2CB6-4061-86BC-958A61D713BE}"/>
+    <hyperlink ref="I24" r:id="rId31" xr:uid="{D635069F-892A-4F1F-8550-500CBD57C42A}"/>
+    <hyperlink ref="L23" r:id="rId32" tooltip="2889133" display="https://uk.farnell.com/vishay/bat85s-tap/diode-schottky-aec-q101-30v-do/dp/2889133?st=bat85" xr:uid="{18F3B860-1AAD-4C5B-BD94-B85954AE7BCF}"/>
+    <hyperlink ref="I26" r:id="rId33" xr:uid="{B2EB5659-CB87-4BB3-8D5A-9C7B2409CC19}"/>
+    <hyperlink ref="I23" r:id="rId34" xr:uid="{2BA0131D-28BF-4B2D-98A8-13B8FD5B1EF5}"/>
+    <hyperlink ref="L21" r:id="rId35" display="https://uk.farnell.com/molex/503398-1892/connector-micro-sd-8pos/dp/2358234?st=5033981892" xr:uid="{11D74044-851C-44EA-91AC-722C6CFB6B3E}"/>
+    <hyperlink ref="I27" r:id="rId36" xr:uid="{2D1FA75B-D9CA-4B13-9AB8-0C3547D07D4A}"/>
+    <hyperlink ref="L27" r:id="rId37" xr:uid="{6CE39B34-9E28-4E0B-8AFF-04670F4E0343}"/>
+    <hyperlink ref="I30" r:id="rId38" xr:uid="{35148EC9-0BBC-4B0C-AAFE-047F71F4E110}"/>
+    <hyperlink ref="I28" r:id="rId39" xr:uid="{AE824952-DBA2-482B-9BC1-1C60443820F2}"/>
+    <hyperlink ref="I32" r:id="rId40" xr:uid="{3DF2667A-C25F-4862-BD28-16FE9FB53834}"/>
+    <hyperlink ref="I29" r:id="rId41" xr:uid="{2F348C2D-AF2B-4DF9-8037-9842338891DE}"/>
+    <hyperlink ref="I34" r:id="rId42" xr:uid="{9BFEF78D-6B49-4504-8ADB-FC6453F0A13A}"/>
+    <hyperlink ref="I33" r:id="rId43" xr:uid="{6BFCB960-4BC4-4AE7-84CC-EF1CFA05B512}"/>
+    <hyperlink ref="I13" r:id="rId44" tooltip="Click to view additional information on this product." xr:uid="{D073EBC7-F736-4CCE-9903-05965C4089DE}"/>
+    <hyperlink ref="I12" r:id="rId45" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/3M-Electronic-Solutions-Division/4816-3000-CP?qs=sGAEpiMZZMs%2FSh%2Fkjph1tvt1%2FmEPT%2FXo2MaLGaLrmns%3D" xr:uid="{110F6884-1DF7-4F57-806C-4EDE39B930B4}"/>
+    <hyperlink ref="I11" r:id="rId46" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/3M-Electronic-Solutions-Division/4820-3000-CP?qs=sGAEpiMZZMs%2FSh%2Fkjph1tvt1%2FmEPT%2FXoGLwqMMa088g%3D" xr:uid="{19C30A73-5D3F-4B86-8369-F9B8DC755041}"/>
+    <hyperlink ref="I37" r:id="rId47" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/SanDisk/SDSDQAF3-008G-I?qs=sGAEpiMZZMtyMAXUUxCBE5IlUgcznewuII5iIueKP0p3215DGin%2Fpg%3D%3D" xr:uid="{1EADA45E-12D0-466C-97A1-D43608EB28DD}"/>
+    <hyperlink ref="I36" r:id="rId48" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/ROBOTIS/903-0058-000?qs=sGAEpiMZZMve4%2FbfQkoj%252BAsyQJpshgj7rMaVzceycow%3D" xr:uid="{81304EC3-CBD1-42AA-9761-BC59FFC325EE}"/>
+    <hyperlink ref="I35" r:id="rId49" tooltip="Click to view additional information on this product." display="https://www.mouser.co.uk/ProductDetail/RAF-Electronic-Hardware/M1265-2545-N?qs=sGAEpiMZZMv2WiXdFcmpiEsCM5xSt%2Fxk" xr:uid="{5D20D5BB-959D-47FB-870B-95BC22A83998}"/>
+    <hyperlink ref="I8" r:id="rId50" display="https://www.mouser.co.uk/ProductDetail/595-SN74HCT74N" xr:uid="{5BF8413D-438B-4996-A00A-5E2B2F4180C9}"/>
+    <hyperlink ref="L9" r:id="rId51" display="https://uk.farnell.com/texas-instruments/sn74hct74n/ic-flip-flop-2-circuits/dp/1470823?MER=sy-me-pd-mi-alte&amp;st=74hct74" xr:uid="{5750A802-3DD7-4FD1-BA5B-66CBCED46A4F}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId51"/>
+  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId52"/>
 </worksheet>
 </file>
</xml_diff>